<commit_message>
All tests work again.
</commit_message>
<xml_diff>
--- a/inst/extdata/Machines - Data/Charcoal_stoves/Charcoal_stoves.xlsx
+++ b/inst/extdata/Machines - Data/Charcoal_stoves/Charcoal_stoves.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6F5067-51F8-884B-B242-EC5139375B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06918A00-7349-B94F-BADE-BF62DE6F6355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -518,7 +518,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -619,6 +619,9 @@
       </c>
       <c r="G4" s="6" t="s">
         <v>20</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.20099155835454899</v>
       </c>
       <c r="I4" s="6">
         <v>0.20099155835454899</v>
@@ -727,21 +730,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010060B7F65646EC444FB25DA4F5E743F4A7" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d7f09569f4a64415a488fee814f89e9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="77d41baf-5ecc-4842-ba36-0ed33caf7049" xmlns:ns4="83e0870f-5ab0-41af-b2c4-f358cb535498" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8efd8f378c7a4511217f3fc9a2a42926" ns3:_="" ns4:_="">
     <xsd:import namespace="77d41baf-5ecc-4842-ba36-0ed33caf7049"/>
@@ -958,32 +946,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF083C1D-CE62-48EF-BAF9-9D27C80F6E5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="83e0870f-5ab0-41af-b2c4-f358cb535498"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="77d41baf-5ecc-4842-ba36-0ed33caf7049"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D57BA165-9822-445B-B328-4F06AD982831}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F97C2014-63BC-4AD0-B7B7-B33C587EA9A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1000,4 +978,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D57BA165-9822-445B-B328-4F06AD982831}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF083C1D-CE62-48EF-BAF9-9D27C80F6E5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="83e0870f-5ab0-41af-b2c4-f358cb535498"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="77d41baf-5ecc-4842-ba36-0ed33caf7049"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>